<commit_message>
Found and fixed crazy gap problem
</commit_message>
<xml_diff>
--- a/Sim-alpha5 - l = 1, m = 0.9.xlsx
+++ b/Sim-alpha5 - l = 1, m = 0.9.xlsx
@@ -598,7 +598,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -607,26 +607,16 @@
             <c:v>Leader</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1006,7 +996,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1015,26 +1005,16 @@
             <c:v>Car 2</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1414,7 +1394,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1423,26 +1403,16 @@
             <c:v>Car 3</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1822,7 +1792,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1832,11 +1802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="349304912"/>
-        <c:axId val="349304520"/>
+        <c:axId val="361068744"/>
+        <c:axId val="361069528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="349304912"/>
+        <c:axId val="361068744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1893,12 +1863,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349304520"/>
+        <c:crossAx val="361069528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="349304520"/>
+        <c:axId val="361069528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1925,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349304912"/>
+        <c:crossAx val="361068744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>